<commit_message>
update the documents, create test data for master data
</commit_message>
<xml_diff>
--- a/doc/tasks/tasks_1_0.xlsx
+++ b/doc/tasks/tasks_1_0.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="55">
   <si>
     <t>Task ID</t>
   </si>
@@ -157,6 +157,30 @@
   </si>
   <si>
     <t>Unit Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        3.1.2</t>
+  </si>
+  <si>
+    <t>Transaction Data Test Case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.2</t>
+  </si>
+  <si>
+    <t>Core test data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        3.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        3.2.2</t>
+  </si>
+  <si>
+    <t>Master Data Test Data</t>
+  </si>
+  <si>
+    <t>Transaction Data Test Data</t>
   </si>
 </sst>
 </file>
@@ -274,8 +298,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0">
-  <autoFilter ref="A1:F19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F23" totalsRowShown="0">
+  <autoFilter ref="A1:F23"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Task ID" dataDxfId="2"/>
     <tableColumn id="2" name="Task Description" dataDxfId="1"/>
@@ -575,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +975,7 @@
         <v>45</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
         <v>19</v>
@@ -960,6 +984,86 @@
         <v>25</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Master data store & load
</commit_message>
<xml_diff>
--- a/doc/tasks/tasks_1_0.xlsx
+++ b/doc/tasks/tasks_1_0.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="71">
   <si>
     <t>Task ID</t>
   </si>
@@ -181,6 +181,54 @@
   </si>
   <si>
     <t>Transaction Data Test Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            3.1.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            3.1.1.2</t>
+  </si>
+  <si>
+    <t>Master Data Test Case - store</t>
+  </si>
+  <si>
+    <t>Master Data Test Case - load</t>
+  </si>
+  <si>
+    <t>Master Data Test Case - create/remove entity</t>
+  </si>
+  <si>
+    <t>G/L account Group master data development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            2.2.1.4</t>
+  </si>
+  <si>
+    <t>Vendor master data development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            2.2.1.5</t>
+  </si>
+  <si>
+    <t>Customer master data development</t>
+  </si>
+  <si>
+    <t>Bank Key master data development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            2.2.1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            2.2.1.7</t>
+  </si>
+  <si>
+    <t>Bank Account master data development</t>
+  </si>
+  <si>
+    <t>Business Area master data development</t>
+  </si>
+  <si>
+    <t>transaction data</t>
   </si>
 </sst>
 </file>
@@ -227,11 +275,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -248,7 +294,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
     <dxf>
       <font>
         <b val="0"/>
@@ -265,6 +311,47 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -298,11 +385,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F23" totalsRowShown="0">
-  <autoFilter ref="A1:F23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F32" totalsRowShown="0">
+  <autoFilter ref="A1:F32"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Task ID" dataDxfId="2"/>
-    <tableColumn id="2" name="Task Description" dataDxfId="1"/>
+    <tableColumn id="1" name="Task ID" dataDxfId="6"/>
+    <tableColumn id="2" name="Task Description" dataDxfId="5"/>
     <tableColumn id="3" name="Status" dataDxfId="0"/>
     <tableColumn id="4" name="Type"/>
     <tableColumn id="5" name="Start Version"/>
@@ -599,26 +686,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -633,132 +720,141 @@
       <c r="F1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -767,303 +863,490 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="35.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="E9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="35.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="1"/>
-      <c r="E16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="D23" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="E23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Document entry finish. Reports function start
</commit_message>
<xml_diff>
--- a/doc/tasks/tasks_1_0.xlsx
+++ b/doc/tasks/tasks_1_0.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="103">
   <si>
     <t>Task ID</t>
   </si>
@@ -150,9 +150,6 @@
     <t xml:space="preserve">    3.2</t>
   </si>
   <si>
-    <t>Core test data</t>
-  </si>
-  <si>
     <t xml:space="preserve">        3.2.1</t>
   </si>
   <si>
@@ -243,13 +240,91 @@
     <t xml:space="preserve">            2.2.2.7</t>
   </si>
   <si>
-    <t>Transaction data</t>
-  </si>
-  <si>
     <t xml:space="preserve">        2.2.4</t>
   </si>
   <si>
     <t>Entry data customizing</t>
+  </si>
+  <si>
+    <t>Reverse</t>
+  </si>
+  <si>
+    <t>Transaction data(Head Entity &amp; Item Entity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            2.2.3.1</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>General Entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            2.2.3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            2.2.3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            2.2.3.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            2.2.3.5</t>
+  </si>
+  <si>
+    <t>Customer invoice entry</t>
+  </si>
+  <si>
+    <t>Vendor invoice entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            2.2.3.6</t>
+  </si>
+  <si>
+    <t>G/L entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            3.1.2.3</t>
+  </si>
+  <si>
+    <t>Transaction Data Test Case - customer invoice entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            3.1.2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            3.1.2.5</t>
+  </si>
+  <si>
+    <t>Transaction Data Test Case - vendor invoice entry</t>
+  </si>
+  <si>
+    <t>Transaction Data Test Case - g/l entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        2.2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        2.2.6</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            2.2.6.1</t>
+  </si>
+  <si>
+    <t>G/L account balance report</t>
+  </si>
+  <si>
+    <t>Report test data</t>
+  </si>
+  <si>
+    <t>G/L account balance report data</t>
   </si>
 </sst>
 </file>
@@ -366,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F37" totalsRowShown="0">
-  <autoFilter ref="A1:F37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F49" totalsRowShown="0">
+  <autoFilter ref="A1:F49"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Task ID" dataDxfId="2"/>
     <tableColumn id="2" name="Task Description" dataDxfId="1"/>
@@ -667,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +948,7 @@
     </row>
     <row r="10" spans="1:8" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>32</v>
@@ -893,7 +968,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
@@ -913,7 +988,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>34</v>
@@ -933,7 +1008,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>35</v>
@@ -953,7 +1028,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>33</v>
@@ -973,7 +1048,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>26</v>
@@ -993,10 +1068,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>8</v>
@@ -1013,10 +1088,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>8</v>
@@ -1033,10 +1108,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>8</v>
@@ -1053,10 +1128,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>8</v>
@@ -1073,10 +1148,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>8</v>
@@ -1093,10 +1168,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>8</v>
@@ -1113,13 +1188,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
         <v>16</v>
@@ -1133,43 +1208,76 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="A24" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="A25" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>40</v>
+        <v>84</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>24</v>
@@ -1180,16 +1288,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>24</v>
@@ -1200,16 +1308,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>24</v>
@@ -1220,16 +1328,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>8</v>
+        <v>75</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>24</v>
@@ -1240,16 +1348,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>24</v>
@@ -1260,16 +1368,16 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>8</v>
+        <v>98</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>24</v>
@@ -1280,16 +1388,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>24</v>
@@ -1300,13 +1408,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>62</v>
+        <v>18</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
         <v>19</v>
@@ -1320,10 +1428,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>5</v>
@@ -1340,10 +1448,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>8</v>
@@ -1360,10 +1468,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>8</v>
@@ -1380,10 +1488,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>8</v>
@@ -1395,6 +1503,246 @@
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modify entry doc. modify G/L account master data test data.
</commit_message>
<xml_diff>
--- a/doc/tasks/tasks_1_0.xlsx
+++ b/doc/tasks/tasks_1_0.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="107">
   <si>
     <t>Task ID</t>
   </si>
@@ -84,9 +84,6 @@
     <t xml:space="preserve">    2.2</t>
   </si>
   <si>
-    <t>Establish the android project</t>
-  </si>
-  <si>
     <t>Android Development</t>
   </si>
   <si>
@@ -325,6 +322,21 @@
   </si>
   <si>
     <t>G/L account balance report data</t>
+  </si>
+  <si>
+    <t>Android UI Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        2.1.1</t>
+  </si>
+  <si>
+    <t>Entry view design</t>
+  </si>
+  <si>
+    <t>Entry view development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        1.3.1</t>
   </si>
 </sst>
 </file>
@@ -441,8 +453,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F49" totalsRowShown="0">
-  <autoFilter ref="A1:F49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F54" totalsRowShown="0">
+  <autoFilter ref="A1:F54"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Task ID" dataDxfId="2"/>
     <tableColumn id="2" name="Task Description" dataDxfId="1"/>
@@ -742,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,10 +783,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -794,10 +806,10 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
@@ -817,10 +829,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
         <v>17</v>
@@ -834,16 +846,16 @@
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -860,78 +872,56 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="35.25" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
@@ -940,118 +930,85 @@
         <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="35.25" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="35.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>33</v>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>63</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
@@ -1060,18 +1017,18 @@
         <v>16</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>8</v>
@@ -1080,18 +1037,18 @@
         <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>8</v>
@@ -1100,18 +1057,18 @@
         <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>8</v>
@@ -1120,18 +1077,18 @@
         <v>16</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>8</v>
@@ -1140,18 +1097,18 @@
         <v>16</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>8</v>
@@ -1160,18 +1117,18 @@
         <v>16</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>8</v>
@@ -1180,18 +1137,18 @@
         <v>16</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>8</v>
@@ -1200,18 +1157,18 @@
         <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>8</v>
@@ -1220,18 +1177,18 @@
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>8</v>
@@ -1240,18 +1197,18 @@
         <v>16</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>8</v>
@@ -1260,18 +1217,18 @@
         <v>16</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>8</v>
@@ -1280,18 +1237,18 @@
         <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>87</v>
+        <v>62</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>8</v>
@@ -1300,258 +1257,258 @@
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>17</v>
+        <v>79</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D29" t="s">
         <v>16</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>5</v>
+        <v>85</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D31" t="s">
         <v>16</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>5</v>
+        <v>86</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D32" t="s">
         <v>16</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>40</v>
+        <v>87</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>5</v>
+        <v>74</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D38" t="s">
         <v>19</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D39" t="s">
         <v>19</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>8</v>
@@ -1560,18 +1517,18 @@
         <v>19</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>8</v>
@@ -1580,18 +1537,18 @@
         <v>19</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>8</v>
@@ -1600,18 +1557,18 @@
         <v>19</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>8</v>
@@ -1620,18 +1577,18 @@
         <v>19</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>8</v>
@@ -1640,78 +1597,78 @@
         <v>19</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D45" t="s">
         <v>19</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
         <v>19</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
         <v>19</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>8</v>
@@ -1720,18 +1677,18 @@
         <v>19</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>8</v>
@@ -1740,10 +1697,110 @@
         <v>19</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>